<commit_message>
Added filtering so that the inputs are protected
</commit_message>
<xml_diff>
--- a/house_map.xlsx
+++ b/house_map.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Devara Mana Sajja</t>
   </si>
@@ -57,13 +57,6 @@
 Computer room sajjaa</t>
   </si>
   <si>
-    <t>Ram room sajjaa</t>
-  </si>
-  <si>
-    <t>Sridhara
-No 10 Passage</t>
-  </si>
-  <si>
     <t>Rishikesha
 No. 10 Toilet</t>
   </si>
@@ -98,6 +91,26 @@
   <si>
     <t>Adhoskshajaa
 Aravind Room Sajja</t>
+  </si>
+  <si>
+    <t>Adhokshaja
+Oota Room Sajjaa</t>
+  </si>
+  <si>
+    <t>Narasimha
+AC Room Sajjaa</t>
+  </si>
+  <si>
+    <t>Achyuta
+Washing Room Sajjaa</t>
+  </si>
+  <si>
+    <t>Janardana
+No 10 Passage</t>
+  </si>
+  <si>
+    <t>Upendra
+Ram room sajjaa</t>
   </si>
 </sst>
 </file>
@@ -129,7 +142,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -152,29 +165,142 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -472,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7:Q12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -483,288 +609,300 @@
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
     <col min="13" max="13" width="11.85546875" customWidth="1"/>
     <col min="14" max="14" width="10.85546875" customWidth="1"/>
-    <col min="17" max="17" width="7.140625" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="30" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="13"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="2"/>
+      <c r="O1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="19.5" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="2" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="2" t="s">
+      <c r="K2" s="8"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="19.5" customHeight="1">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="6"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="4"/>
     </row>
     <row r="3" spans="1:17" ht="19.5" customHeight="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="6"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-      <c r="Q4" s="6"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="4"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="6"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="4"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="6"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="2" t="s">
+      <c r="A7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="5"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="5"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="4"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="5"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="2" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="5" t="s">
+      <c r="N10" s="2"/>
+      <c r="O10" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" s="1"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="6"/>
-    </row>
-    <row r="9" spans="1:17">
-      <c r="A9" s="1"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="6"/>
-    </row>
-    <row r="10" spans="1:17">
-      <c r="A10" s="1"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P10" s="4"/>
-      <c r="Q10" s="6"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="4"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="1"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="6"/>
+      <c r="A11" s="5"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="4"/>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="1"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="6"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="G7:I12"/>
-    <mergeCell ref="E7:F9"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="G1:I6"/>
-    <mergeCell ref="J1:L6"/>
-    <mergeCell ref="M1:N6"/>
+  <mergeCells count="24">
+    <mergeCell ref="G2:I6"/>
+    <mergeCell ref="J2:L6"/>
+    <mergeCell ref="M2:N6"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="B1:D6"/>
+    <mergeCell ref="B7:D12"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F3"/>
+    <mergeCell ref="E4:F6"/>
     <mergeCell ref="O1:P6"/>
     <mergeCell ref="Q1:Q6"/>
     <mergeCell ref="Q7:Q12"/>
@@ -772,13 +910,10 @@
     <mergeCell ref="O10:P12"/>
     <mergeCell ref="M10:N12"/>
     <mergeCell ref="J7:L12"/>
-    <mergeCell ref="A1:A6"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="B1:D6"/>
-    <mergeCell ref="B7:D12"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F3"/>
-    <mergeCell ref="E4:F6"/>
+    <mergeCell ref="G7:I12"/>
+    <mergeCell ref="E7:F9"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="E10:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>